<commit_message>
Update Internal Tracking Sheet TCS (LAPTOP-ANV4TEJD's conflicted copy 2021-10-30).xlsx
</commit_message>
<xml_diff>
--- a/gameoflife-acceptance-tests/Internal Tracking Sheet TCS (LAPTOP-ANV4TEJD's conflicted copy 2021-10-30).xlsx
+++ b/gameoflife-acceptance-tests/Internal Tracking Sheet TCS (LAPTOP-ANV4TEJD's conflicted copy 2021-10-30).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOHN PRAKASH\OneDrive\Desktop\SR Software solutions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOHN PRAKASH\OneDrive\Documents\GitHub\Jenkins\gameoflife-acceptance-tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753A82CF-C5A5-4E0E-A3DA-12E59609A361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9DA246-5F01-4F04-BC0C-01D0DBD87151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="11" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Email id" sheetId="10" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="Sheet1" sheetId="17" r:id="rId13"/>
     <sheet name="Nov- Dec Applications" sheetId="14" r:id="rId14"/>
     <sheet name="Jan 2022" sheetId="16" r:id="rId15"/>
+    <sheet name="Sheet2" sheetId="18" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'July Applications'!$A$1:$M$67</definedName>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2110" uniqueCount="915">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2111" uniqueCount="916">
   <si>
     <t>No</t>
   </si>
@@ -2937,6 +2938,9 @@
   </si>
   <si>
     <t>Not attended</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fd</t>
   </si>
 </sst>
 </file>
@@ -6564,8 +6568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E890015-DF43-4B53-B209-D42A5349F3E3}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7196,6 +7200,24 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA5E676-30BF-4456-8AB8-7B9202AB306A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>915</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>